<commit_message>
added basic joystick control
</commit_message>
<xml_diff>
--- a/DisplayTable.xlsx
+++ b/DisplayTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renaudlh\Code\greenhouse-esp32\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33D4383-D1D9-4EDC-A82B-16ABF2B9B342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC4CDE5-6321-47AD-B5AB-C07E74DECD16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-495" windowWidth="29040" windowHeight="15720" xr2:uid="{9640423A-1E3F-433A-99EE-B51C040EA3B4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="38">
   <si>
     <t>E</t>
   </si>
@@ -536,7 +536,7 @@
   <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,34 +947,22 @@
       <c r="G12" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="H12" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="I12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M12" s="1" t="s">
-        <v>20</v>
+      <c r="K12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
+        <v>6</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="R12" s="1">
-        <v>0</v>
-      </c>
-      <c r="S12" s="1">
-        <v>6</v>
-      </c>
-      <c r="T12" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1000,37 +988,25 @@
       <c r="G13" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="H13" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="I13" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>31</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="R13" s="1">
-        <v>0</v>
-      </c>
-      <c r="S13" s="1">
-        <v>0</v>
-      </c>
-      <c r="T13" s="1" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>